<commit_message>
Rewriting test cases to clarify the steps in them
</commit_message>
<xml_diff>
--- a/TestCases/Back End/CreateAssessment-BackEnd-Director.xlsx
+++ b/TestCases/Back End/CreateAssessment-BackEnd-Director.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18805"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F1186400-FCA4-4BC8-AF52-256EAD50FA56}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{52F61FCE-2262-4456-87A9-8AB24FB84F66}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{F1186400-FCA4-4BC8-AF52-256EAD50FA56}" xr6:coauthVersionLast="26" xr6:coauthVersionMax="26" xr10:uidLastSave="{F27C772B-8FEE-4FCF-B8EF-9254A76DCFF5}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,12 +15,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Role: Director</t>
   </si>
   <si>
-    <t>Test Case: Testing to see if creating an assessment adds it to the database</t>
+    <t>Test Case: Testing to see if creating assessments reaches data base with no errors</t>
   </si>
   <si>
     <t>Steps</t>
@@ -35,16 +35,34 @@
     <t>Pass/Fail</t>
   </si>
   <si>
-    <t>Step 1: While logged out, try to create an assessment</t>
-  </si>
-  <si>
-    <t>I am redirected to the login screen</t>
-  </si>
-  <si>
-    <t>Step 2: Log in and from the dashboard go to "Create Assessment" and create an assessment for an employee</t>
-  </si>
-  <si>
-    <t>The assessment is added to the database</t>
+    <t>Step 1: While logged out go to the create assessment page</t>
+  </si>
+  <si>
+    <t>I am returned to the login page</t>
+  </si>
+  <si>
+    <t>Step 2: Login as a the appropriate and go to the "create assessment" page</t>
+  </si>
+  <si>
+    <t>I am redirected to the create assessment page</t>
+  </si>
+  <si>
+    <t>Step 3: Fill out a assessment for an employee</t>
+  </si>
+  <si>
+    <t>A new assessment will be added to the database on that employee</t>
+  </si>
+  <si>
+    <t>Step 5: Leave Certain fields that are required blank (everything but comments are required)</t>
+  </si>
+  <si>
+    <t>Error text pop up saying that some of the fields have been left blank</t>
+  </si>
+  <si>
+    <t>Step 6: Create an assessment for the current role logged in</t>
+  </si>
+  <si>
+    <t>I am denied access to this</t>
   </si>
 </sst>
 </file>
@@ -394,9 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -445,9 +461,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="56.25" customHeight="1"/>
-    <row r="5" spans="1:6" ht="58.5" customHeight="1"/>
-    <row r="6" spans="1:6" ht="60.75" customHeight="1"/>
+    <row r="4" spans="1:6" ht="56.25" customHeight="1">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="58.5" customHeight="1">
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="60.75" customHeight="1">
+      <c r="C6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
     <row r="7" spans="1:6" ht="60.75" customHeight="1">
       <c r="F7" s="2"/>
     </row>

</xml_diff>